<commit_message>
Added documentation to functions and readme, created igsights_env.yml, updated backups.
</commit_message>
<xml_diff>
--- a/data/cleaned_data/daily_actions_metrics.xlsx
+++ b/data/cleaned_data/daily_actions_metrics.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I313"/>
+  <dimension ref="A1:I433"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12200,7 +12200,7 @@
         <v>2357</v>
       </c>
       <c r="D302" s="3" t="n">
-        <v>45779.39788771026</v>
+        <v>45779.39788770834</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -12239,7 +12239,7 @@
         <v>1</v>
       </c>
       <c r="D303" s="3" t="n">
-        <v>45779.39788771026</v>
+        <v>45779.39788770834</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -12278,7 +12278,7 @@
         <v>83</v>
       </c>
       <c r="D304" s="3" t="n">
-        <v>45779.39788771026</v>
+        <v>45779.39788770834</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -12317,7 +12317,7 @@
         <v>271</v>
       </c>
       <c r="D305" s="3" t="n">
-        <v>45779.39788771026</v>
+        <v>45779.39788770834</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -12356,7 +12356,7 @@
         <v>221</v>
       </c>
       <c r="D306" s="3" t="n">
-        <v>45779.39788771026</v>
+        <v>45779.39788770834</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -12395,7 +12395,7 @@
         <v>10</v>
       </c>
       <c r="D307" s="3" t="n">
-        <v>45779.39788771026</v>
+        <v>45779.39788770834</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -12434,7 +12434,7 @@
         <v>13</v>
       </c>
       <c r="D308" s="3" t="n">
-        <v>45779.39788771026</v>
+        <v>45779.39788770834</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -12473,7 +12473,7 @@
         <v>25</v>
       </c>
       <c r="D309" s="3" t="n">
-        <v>45779.39788771026</v>
+        <v>45779.39788770834</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -12512,7 +12512,7 @@
         <v>2</v>
       </c>
       <c r="D310" s="3" t="n">
-        <v>45779.39788771026</v>
+        <v>45779.39788770834</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -12551,7 +12551,7 @@
         <v>4128</v>
       </c>
       <c r="D311" s="3" t="n">
-        <v>45779.39788771026</v>
+        <v>45779.39788770834</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -12590,7 +12590,7 @@
         <v>0</v>
       </c>
       <c r="D312" s="3" t="n">
-        <v>45779.39788771026</v>
+        <v>45779.39788770834</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -12629,7 +12629,7 @@
         <v>0</v>
       </c>
       <c r="D313" s="3" t="n">
-        <v>45779.39788771026</v>
+        <v>45779.39788770834</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -12650,6 +12650,4686 @@
       <c r="I313" t="inlineStr">
         <is>
           <t>09:32:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>reach</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Accounts reached</t>
+        </is>
+      </c>
+      <c r="C314" t="n">
+        <v>2273</v>
+      </c>
+      <c r="D314" s="3" t="n">
+        <v>45780.39801960648</v>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>2025-05-03</t>
+        </is>
+      </c>
+      <c r="F314" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G314" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H314" t="n">
+        <v>3</v>
+      </c>
+      <c r="I314" t="inlineStr">
+        <is>
+          <t>09:33:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>website_clicks</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Website link taps</t>
+        </is>
+      </c>
+      <c r="C315" t="n">
+        <v>0</v>
+      </c>
+      <c r="D315" s="3" t="n">
+        <v>45780.39801960648</v>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>2025-05-03</t>
+        </is>
+      </c>
+      <c r="F315" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G315" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H315" t="n">
+        <v>3</v>
+      </c>
+      <c r="I315" t="inlineStr">
+        <is>
+          <t>09:33:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>profile_views</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Profile visits</t>
+        </is>
+      </c>
+      <c r="C316" t="n">
+        <v>85</v>
+      </c>
+      <c r="D316" s="3" t="n">
+        <v>45780.39801960648</v>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>2025-05-03</t>
+        </is>
+      </c>
+      <c r="F316" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G316" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H316" t="n">
+        <v>3</v>
+      </c>
+      <c r="I316" t="inlineStr">
+        <is>
+          <t>09:33:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>total_interactions</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Content interactions</t>
+        </is>
+      </c>
+      <c r="C317" t="n">
+        <v>266</v>
+      </c>
+      <c r="D317" s="3" t="n">
+        <v>45780.39801960648</v>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>2025-05-03</t>
+        </is>
+      </c>
+      <c r="F317" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G317" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H317" t="n">
+        <v>3</v>
+      </c>
+      <c r="I317" t="inlineStr">
+        <is>
+          <t>09:33:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>likes</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Likes</t>
+        </is>
+      </c>
+      <c r="C318" t="n">
+        <v>217</v>
+      </c>
+      <c r="D318" s="3" t="n">
+        <v>45780.39801960648</v>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>2025-05-03</t>
+        </is>
+      </c>
+      <c r="F318" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G318" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H318" t="n">
+        <v>3</v>
+      </c>
+      <c r="I318" t="inlineStr">
+        <is>
+          <t>09:33:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="C319" t="n">
+        <v>4</v>
+      </c>
+      <c r="D319" s="3" t="n">
+        <v>45780.39801960648</v>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>2025-05-03</t>
+        </is>
+      </c>
+      <c r="F319" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G319" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H319" t="n">
+        <v>3</v>
+      </c>
+      <c r="I319" t="inlineStr">
+        <is>
+          <t>09:33:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>shares</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Shares</t>
+        </is>
+      </c>
+      <c r="C320" t="n">
+        <v>13</v>
+      </c>
+      <c r="D320" s="3" t="n">
+        <v>45780.39801960648</v>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>2025-05-03</t>
+        </is>
+      </c>
+      <c r="F320" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G320" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H320" t="n">
+        <v>3</v>
+      </c>
+      <c r="I320" t="inlineStr">
+        <is>
+          <t>09:33:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>saves</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Saves</t>
+        </is>
+      </c>
+      <c r="C321" t="n">
+        <v>28</v>
+      </c>
+      <c r="D321" s="3" t="n">
+        <v>45780.39801960648</v>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>2025-05-03</t>
+        </is>
+      </c>
+      <c r="F321" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G321" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H321" t="n">
+        <v>3</v>
+      </c>
+      <c r="I321" t="inlineStr">
+        <is>
+          <t>09:33:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>replies</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Replies</t>
+        </is>
+      </c>
+      <c r="C322" t="n">
+        <v>4</v>
+      </c>
+      <c r="D322" s="3" t="n">
+        <v>45780.39801960648</v>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>2025-05-03</t>
+        </is>
+      </c>
+      <c r="F322" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G322" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H322" t="n">
+        <v>3</v>
+      </c>
+      <c r="I322" t="inlineStr">
+        <is>
+          <t>09:33:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>views</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Views</t>
+        </is>
+      </c>
+      <c r="C323" t="n">
+        <v>3842</v>
+      </c>
+      <c r="D323" s="3" t="n">
+        <v>45780.39801960648</v>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>2025-05-03</t>
+        </is>
+      </c>
+      <c r="F323" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G323" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H323" t="n">
+        <v>3</v>
+      </c>
+      <c r="I323" t="inlineStr">
+        <is>
+          <t>09:33:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>follows_and_unfollows</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Follows and unfollows</t>
+        </is>
+      </c>
+      <c r="C324" t="n">
+        <v>0</v>
+      </c>
+      <c r="D324" s="3" t="n">
+        <v>45780.39801960648</v>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>2025-05-03</t>
+        </is>
+      </c>
+      <c r="F324" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G324" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H324" t="n">
+        <v>3</v>
+      </c>
+      <c r="I324" t="inlineStr">
+        <is>
+          <t>09:33:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>profile_links_taps</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Profile links taps</t>
+        </is>
+      </c>
+      <c r="C325" t="n">
+        <v>0</v>
+      </c>
+      <c r="D325" s="3" t="n">
+        <v>45780.39801960648</v>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>2025-05-03</t>
+        </is>
+      </c>
+      <c r="F325" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G325" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H325" t="n">
+        <v>3</v>
+      </c>
+      <c r="I325" t="inlineStr">
+        <is>
+          <t>09:33:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>reach</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Accounts reached</t>
+        </is>
+      </c>
+      <c r="C326" t="n">
+        <v>1251</v>
+      </c>
+      <c r="D326" s="3" t="n">
+        <v>45781.3978862037</v>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="F326" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G326" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H326" t="n">
+        <v>4</v>
+      </c>
+      <c r="I326" t="inlineStr">
+        <is>
+          <t>09:32:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>website_clicks</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Website link taps</t>
+        </is>
+      </c>
+      <c r="C327" t="n">
+        <v>0</v>
+      </c>
+      <c r="D327" s="3" t="n">
+        <v>45781.3978862037</v>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="F327" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G327" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H327" t="n">
+        <v>4</v>
+      </c>
+      <c r="I327" t="inlineStr">
+        <is>
+          <t>09:32:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>profile_views</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Profile visits</t>
+        </is>
+      </c>
+      <c r="C328" t="n">
+        <v>69</v>
+      </c>
+      <c r="D328" s="3" t="n">
+        <v>45781.3978862037</v>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="F328" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G328" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H328" t="n">
+        <v>4</v>
+      </c>
+      <c r="I328" t="inlineStr">
+        <is>
+          <t>09:32:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>total_interactions</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Content interactions</t>
+        </is>
+      </c>
+      <c r="C329" t="n">
+        <v>287</v>
+      </c>
+      <c r="D329" s="3" t="n">
+        <v>45781.3978862037</v>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="F329" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G329" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H329" t="n">
+        <v>4</v>
+      </c>
+      <c r="I329" t="inlineStr">
+        <is>
+          <t>09:32:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>likes</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Likes</t>
+        </is>
+      </c>
+      <c r="C330" t="n">
+        <v>190</v>
+      </c>
+      <c r="D330" s="3" t="n">
+        <v>45781.3978862037</v>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="F330" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G330" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H330" t="n">
+        <v>4</v>
+      </c>
+      <c r="I330" t="inlineStr">
+        <is>
+          <t>09:32:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="C331" t="n">
+        <v>9</v>
+      </c>
+      <c r="D331" s="3" t="n">
+        <v>45781.3978862037</v>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="F331" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G331" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H331" t="n">
+        <v>4</v>
+      </c>
+      <c r="I331" t="inlineStr">
+        <is>
+          <t>09:32:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>shares</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Shares</t>
+        </is>
+      </c>
+      <c r="C332" t="n">
+        <v>3</v>
+      </c>
+      <c r="D332" s="3" t="n">
+        <v>45781.3978862037</v>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="F332" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G332" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H332" t="n">
+        <v>4</v>
+      </c>
+      <c r="I332" t="inlineStr">
+        <is>
+          <t>09:32:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>saves</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Saves</t>
+        </is>
+      </c>
+      <c r="C333" t="n">
+        <v>81</v>
+      </c>
+      <c r="D333" s="3" t="n">
+        <v>45781.3978862037</v>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="F333" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G333" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H333" t="n">
+        <v>4</v>
+      </c>
+      <c r="I333" t="inlineStr">
+        <is>
+          <t>09:32:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>replies</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Replies</t>
+        </is>
+      </c>
+      <c r="C334" t="n">
+        <v>4</v>
+      </c>
+      <c r="D334" s="3" t="n">
+        <v>45781.3978862037</v>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="F334" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G334" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H334" t="n">
+        <v>4</v>
+      </c>
+      <c r="I334" t="inlineStr">
+        <is>
+          <t>09:32:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>views</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Views</t>
+        </is>
+      </c>
+      <c r="C335" t="n">
+        <v>2764</v>
+      </c>
+      <c r="D335" s="3" t="n">
+        <v>45781.3978862037</v>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="F335" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G335" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H335" t="n">
+        <v>4</v>
+      </c>
+      <c r="I335" t="inlineStr">
+        <is>
+          <t>09:32:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>follows_and_unfollows</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Follows and unfollows</t>
+        </is>
+      </c>
+      <c r="C336" t="n">
+        <v>0</v>
+      </c>
+      <c r="D336" s="3" t="n">
+        <v>45781.3978862037</v>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="F336" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G336" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H336" t="n">
+        <v>4</v>
+      </c>
+      <c r="I336" t="inlineStr">
+        <is>
+          <t>09:32:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>profile_links_taps</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Profile links taps</t>
+        </is>
+      </c>
+      <c r="C337" t="n">
+        <v>0</v>
+      </c>
+      <c r="D337" s="3" t="n">
+        <v>45781.3978862037</v>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>2025-05-04</t>
+        </is>
+      </c>
+      <c r="F337" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G337" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H337" t="n">
+        <v>4</v>
+      </c>
+      <c r="I337" t="inlineStr">
+        <is>
+          <t>09:32:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>reach</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Accounts reached</t>
+        </is>
+      </c>
+      <c r="C338" t="n">
+        <v>1023</v>
+      </c>
+      <c r="D338" s="3" t="n">
+        <v>45782.40762505787</v>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>2025-05-05</t>
+        </is>
+      </c>
+      <c r="F338" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G338" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H338" t="n">
+        <v>5</v>
+      </c>
+      <c r="I338" t="inlineStr">
+        <is>
+          <t>09:46:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>website_clicks</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Website link taps</t>
+        </is>
+      </c>
+      <c r="C339" t="n">
+        <v>0</v>
+      </c>
+      <c r="D339" s="3" t="n">
+        <v>45782.40762505787</v>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>2025-05-05</t>
+        </is>
+      </c>
+      <c r="F339" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G339" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H339" t="n">
+        <v>5</v>
+      </c>
+      <c r="I339" t="inlineStr">
+        <is>
+          <t>09:46:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>profile_views</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Profile visits</t>
+        </is>
+      </c>
+      <c r="C340" t="n">
+        <v>57</v>
+      </c>
+      <c r="D340" s="3" t="n">
+        <v>45782.40762505787</v>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>2025-05-05</t>
+        </is>
+      </c>
+      <c r="F340" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G340" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H340" t="n">
+        <v>5</v>
+      </c>
+      <c r="I340" t="inlineStr">
+        <is>
+          <t>09:46:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>total_interactions</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Content interactions</t>
+        </is>
+      </c>
+      <c r="C341" t="n">
+        <v>104</v>
+      </c>
+      <c r="D341" s="3" t="n">
+        <v>45782.40762505787</v>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>2025-05-05</t>
+        </is>
+      </c>
+      <c r="F341" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G341" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H341" t="n">
+        <v>5</v>
+      </c>
+      <c r="I341" t="inlineStr">
+        <is>
+          <t>09:46:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>likes</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Likes</t>
+        </is>
+      </c>
+      <c r="C342" t="n">
+        <v>93</v>
+      </c>
+      <c r="D342" s="3" t="n">
+        <v>45782.40762505787</v>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>2025-05-05</t>
+        </is>
+      </c>
+      <c r="F342" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G342" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H342" t="n">
+        <v>5</v>
+      </c>
+      <c r="I342" t="inlineStr">
+        <is>
+          <t>09:46:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="C343" t="n">
+        <v>1</v>
+      </c>
+      <c r="D343" s="3" t="n">
+        <v>45782.40762505787</v>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>2025-05-05</t>
+        </is>
+      </c>
+      <c r="F343" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G343" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H343" t="n">
+        <v>5</v>
+      </c>
+      <c r="I343" t="inlineStr">
+        <is>
+          <t>09:46:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>shares</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Shares</t>
+        </is>
+      </c>
+      <c r="C344" t="n">
+        <v>3</v>
+      </c>
+      <c r="D344" s="3" t="n">
+        <v>45782.40762505787</v>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>2025-05-05</t>
+        </is>
+      </c>
+      <c r="F344" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G344" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H344" t="n">
+        <v>5</v>
+      </c>
+      <c r="I344" t="inlineStr">
+        <is>
+          <t>09:46:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>saves</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Saves</t>
+        </is>
+      </c>
+      <c r="C345" t="n">
+        <v>5</v>
+      </c>
+      <c r="D345" s="3" t="n">
+        <v>45782.40762505787</v>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>2025-05-05</t>
+        </is>
+      </c>
+      <c r="F345" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G345" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H345" t="n">
+        <v>5</v>
+      </c>
+      <c r="I345" t="inlineStr">
+        <is>
+          <t>09:46:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>replies</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Replies</t>
+        </is>
+      </c>
+      <c r="C346" t="n">
+        <v>2</v>
+      </c>
+      <c r="D346" s="3" t="n">
+        <v>45782.40762505787</v>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>2025-05-05</t>
+        </is>
+      </c>
+      <c r="F346" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G346" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H346" t="n">
+        <v>5</v>
+      </c>
+      <c r="I346" t="inlineStr">
+        <is>
+          <t>09:46:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>views</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Views</t>
+        </is>
+      </c>
+      <c r="C347" t="n">
+        <v>2103</v>
+      </c>
+      <c r="D347" s="3" t="n">
+        <v>45782.40762505787</v>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>2025-05-05</t>
+        </is>
+      </c>
+      <c r="F347" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G347" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H347" t="n">
+        <v>5</v>
+      </c>
+      <c r="I347" t="inlineStr">
+        <is>
+          <t>09:46:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>follows_and_unfollows</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Follows and unfollows</t>
+        </is>
+      </c>
+      <c r="C348" t="n">
+        <v>0</v>
+      </c>
+      <c r="D348" s="3" t="n">
+        <v>45782.40762505787</v>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>2025-05-05</t>
+        </is>
+      </c>
+      <c r="F348" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G348" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H348" t="n">
+        <v>5</v>
+      </c>
+      <c r="I348" t="inlineStr">
+        <is>
+          <t>09:46:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>profile_links_taps</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Profile links taps</t>
+        </is>
+      </c>
+      <c r="C349" t="n">
+        <v>0</v>
+      </c>
+      <c r="D349" s="3" t="n">
+        <v>45782.40762505787</v>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>2025-05-05</t>
+        </is>
+      </c>
+      <c r="F349" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G349" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H349" t="n">
+        <v>5</v>
+      </c>
+      <c r="I349" t="inlineStr">
+        <is>
+          <t>09:46:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>reach</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Accounts reached</t>
+        </is>
+      </c>
+      <c r="C350" t="n">
+        <v>866</v>
+      </c>
+      <c r="D350" s="3" t="n">
+        <v>45783.39773483796</v>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="F350" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G350" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H350" t="n">
+        <v>6</v>
+      </c>
+      <c r="I350" t="inlineStr">
+        <is>
+          <t>09:32:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>website_clicks</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Website link taps</t>
+        </is>
+      </c>
+      <c r="C351" t="n">
+        <v>0</v>
+      </c>
+      <c r="D351" s="3" t="n">
+        <v>45783.39773483796</v>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="F351" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G351" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H351" t="n">
+        <v>6</v>
+      </c>
+      <c r="I351" t="inlineStr">
+        <is>
+          <t>09:32:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>profile_views</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Profile visits</t>
+        </is>
+      </c>
+      <c r="C352" t="n">
+        <v>44</v>
+      </c>
+      <c r="D352" s="3" t="n">
+        <v>45783.39773483796</v>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="F352" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G352" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H352" t="n">
+        <v>6</v>
+      </c>
+      <c r="I352" t="inlineStr">
+        <is>
+          <t>09:32:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>total_interactions</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Content interactions</t>
+        </is>
+      </c>
+      <c r="C353" t="n">
+        <v>79</v>
+      </c>
+      <c r="D353" s="3" t="n">
+        <v>45783.39773483796</v>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="F353" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G353" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H353" t="n">
+        <v>6</v>
+      </c>
+      <c r="I353" t="inlineStr">
+        <is>
+          <t>09:32:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>likes</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Likes</t>
+        </is>
+      </c>
+      <c r="C354" t="n">
+        <v>66</v>
+      </c>
+      <c r="D354" s="3" t="n">
+        <v>45783.39773483796</v>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="F354" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G354" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H354" t="n">
+        <v>6</v>
+      </c>
+      <c r="I354" t="inlineStr">
+        <is>
+          <t>09:32:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="C355" t="n">
+        <v>1</v>
+      </c>
+      <c r="D355" s="3" t="n">
+        <v>45783.39773483796</v>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="F355" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G355" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H355" t="n">
+        <v>6</v>
+      </c>
+      <c r="I355" t="inlineStr">
+        <is>
+          <t>09:32:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>shares</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Shares</t>
+        </is>
+      </c>
+      <c r="C356" t="n">
+        <v>3</v>
+      </c>
+      <c r="D356" s="3" t="n">
+        <v>45783.39773483796</v>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="F356" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G356" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H356" t="n">
+        <v>6</v>
+      </c>
+      <c r="I356" t="inlineStr">
+        <is>
+          <t>09:32:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>saves</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Saves</t>
+        </is>
+      </c>
+      <c r="C357" t="n">
+        <v>9</v>
+      </c>
+      <c r="D357" s="3" t="n">
+        <v>45783.39773483796</v>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="F357" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G357" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H357" t="n">
+        <v>6</v>
+      </c>
+      <c r="I357" t="inlineStr">
+        <is>
+          <t>09:32:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>replies</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Replies</t>
+        </is>
+      </c>
+      <c r="C358" t="n">
+        <v>0</v>
+      </c>
+      <c r="D358" s="3" t="n">
+        <v>45783.39773483796</v>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="F358" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G358" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H358" t="n">
+        <v>6</v>
+      </c>
+      <c r="I358" t="inlineStr">
+        <is>
+          <t>09:32:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>views</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Views</t>
+        </is>
+      </c>
+      <c r="C359" t="n">
+        <v>1355</v>
+      </c>
+      <c r="D359" s="3" t="n">
+        <v>45783.39773483796</v>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="F359" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G359" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H359" t="n">
+        <v>6</v>
+      </c>
+      <c r="I359" t="inlineStr">
+        <is>
+          <t>09:32:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>follows_and_unfollows</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Follows and unfollows</t>
+        </is>
+      </c>
+      <c r="C360" t="n">
+        <v>0</v>
+      </c>
+      <c r="D360" s="3" t="n">
+        <v>45783.39773483796</v>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="F360" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G360" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H360" t="n">
+        <v>6</v>
+      </c>
+      <c r="I360" t="inlineStr">
+        <is>
+          <t>09:32:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>profile_links_taps</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Profile links taps</t>
+        </is>
+      </c>
+      <c r="C361" t="n">
+        <v>0</v>
+      </c>
+      <c r="D361" s="3" t="n">
+        <v>45783.39773483796</v>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+      <c r="F361" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G361" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H361" t="n">
+        <v>6</v>
+      </c>
+      <c r="I361" t="inlineStr">
+        <is>
+          <t>09:32:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>reach</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Accounts reached</t>
+        </is>
+      </c>
+      <c r="C362" t="n">
+        <v>1043</v>
+      </c>
+      <c r="D362" s="3" t="n">
+        <v>45784.3976696875</v>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="F362" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G362" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H362" t="n">
+        <v>7</v>
+      </c>
+      <c r="I362" t="inlineStr">
+        <is>
+          <t>09:32:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>website_clicks</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Website link taps</t>
+        </is>
+      </c>
+      <c r="C363" t="n">
+        <v>1</v>
+      </c>
+      <c r="D363" s="3" t="n">
+        <v>45784.3976696875</v>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="F363" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G363" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H363" t="n">
+        <v>7</v>
+      </c>
+      <c r="I363" t="inlineStr">
+        <is>
+          <t>09:32:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>profile_views</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Profile visits</t>
+        </is>
+      </c>
+      <c r="C364" t="n">
+        <v>39</v>
+      </c>
+      <c r="D364" s="3" t="n">
+        <v>45784.3976696875</v>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="F364" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G364" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H364" t="n">
+        <v>7</v>
+      </c>
+      <c r="I364" t="inlineStr">
+        <is>
+          <t>09:32:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>total_interactions</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Content interactions</t>
+        </is>
+      </c>
+      <c r="C365" t="n">
+        <v>175</v>
+      </c>
+      <c r="D365" s="3" t="n">
+        <v>45784.3976696875</v>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="F365" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G365" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H365" t="n">
+        <v>7</v>
+      </c>
+      <c r="I365" t="inlineStr">
+        <is>
+          <t>09:32:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>likes</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Likes</t>
+        </is>
+      </c>
+      <c r="C366" t="n">
+        <v>149</v>
+      </c>
+      <c r="D366" s="3" t="n">
+        <v>45784.3976696875</v>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="F366" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G366" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H366" t="n">
+        <v>7</v>
+      </c>
+      <c r="I366" t="inlineStr">
+        <is>
+          <t>09:32:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="C367" t="n">
+        <v>14</v>
+      </c>
+      <c r="D367" s="3" t="n">
+        <v>45784.3976696875</v>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="F367" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G367" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H367" t="n">
+        <v>7</v>
+      </c>
+      <c r="I367" t="inlineStr">
+        <is>
+          <t>09:32:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>shares</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Shares</t>
+        </is>
+      </c>
+      <c r="C368" t="n">
+        <v>3</v>
+      </c>
+      <c r="D368" s="3" t="n">
+        <v>45784.3976696875</v>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="F368" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G368" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H368" t="n">
+        <v>7</v>
+      </c>
+      <c r="I368" t="inlineStr">
+        <is>
+          <t>09:32:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>saves</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Saves</t>
+        </is>
+      </c>
+      <c r="C369" t="n">
+        <v>8</v>
+      </c>
+      <c r="D369" s="3" t="n">
+        <v>45784.3976696875</v>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="F369" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G369" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H369" t="n">
+        <v>7</v>
+      </c>
+      <c r="I369" t="inlineStr">
+        <is>
+          <t>09:32:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>replies</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Replies</t>
+        </is>
+      </c>
+      <c r="C370" t="n">
+        <v>1</v>
+      </c>
+      <c r="D370" s="3" t="n">
+        <v>45784.3976696875</v>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="F370" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G370" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H370" t="n">
+        <v>7</v>
+      </c>
+      <c r="I370" t="inlineStr">
+        <is>
+          <t>09:32:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>views</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Views</t>
+        </is>
+      </c>
+      <c r="C371" t="n">
+        <v>1909</v>
+      </c>
+      <c r="D371" s="3" t="n">
+        <v>45784.3976696875</v>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="F371" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G371" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H371" t="n">
+        <v>7</v>
+      </c>
+      <c r="I371" t="inlineStr">
+        <is>
+          <t>09:32:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>follows_and_unfollows</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Follows and unfollows</t>
+        </is>
+      </c>
+      <c r="C372" t="n">
+        <v>0</v>
+      </c>
+      <c r="D372" s="3" t="n">
+        <v>45784.3976696875</v>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="F372" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G372" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H372" t="n">
+        <v>7</v>
+      </c>
+      <c r="I372" t="inlineStr">
+        <is>
+          <t>09:32:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>profile_links_taps</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Profile links taps</t>
+        </is>
+      </c>
+      <c r="C373" t="n">
+        <v>0</v>
+      </c>
+      <c r="D373" s="3" t="n">
+        <v>45784.3976696875</v>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>2025-05-07</t>
+        </is>
+      </c>
+      <c r="F373" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G373" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H373" t="n">
+        <v>7</v>
+      </c>
+      <c r="I373" t="inlineStr">
+        <is>
+          <t>09:32:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>reach</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Accounts reached</t>
+        </is>
+      </c>
+      <c r="C374" t="n">
+        <v>1001</v>
+      </c>
+      <c r="D374" s="3" t="n">
+        <v>45785.39820251158</v>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="F374" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G374" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H374" t="n">
+        <v>8</v>
+      </c>
+      <c r="I374" t="inlineStr">
+        <is>
+          <t>09:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>website_clicks</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Website link taps</t>
+        </is>
+      </c>
+      <c r="C375" t="n">
+        <v>0</v>
+      </c>
+      <c r="D375" s="3" t="n">
+        <v>45785.39820251158</v>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="F375" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G375" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H375" t="n">
+        <v>8</v>
+      </c>
+      <c r="I375" t="inlineStr">
+        <is>
+          <t>09:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>profile_views</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Profile visits</t>
+        </is>
+      </c>
+      <c r="C376" t="n">
+        <v>47</v>
+      </c>
+      <c r="D376" s="3" t="n">
+        <v>45785.39820251158</v>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="F376" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G376" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H376" t="n">
+        <v>8</v>
+      </c>
+      <c r="I376" t="inlineStr">
+        <is>
+          <t>09:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>total_interactions</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Content interactions</t>
+        </is>
+      </c>
+      <c r="C377" t="n">
+        <v>118</v>
+      </c>
+      <c r="D377" s="3" t="n">
+        <v>45785.39820251158</v>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="F377" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G377" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H377" t="n">
+        <v>8</v>
+      </c>
+      <c r="I377" t="inlineStr">
+        <is>
+          <t>09:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>likes</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Likes</t>
+        </is>
+      </c>
+      <c r="C378" t="n">
+        <v>105</v>
+      </c>
+      <c r="D378" s="3" t="n">
+        <v>45785.39820251158</v>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="F378" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G378" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H378" t="n">
+        <v>8</v>
+      </c>
+      <c r="I378" t="inlineStr">
+        <is>
+          <t>09:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="C379" t="n">
+        <v>7</v>
+      </c>
+      <c r="D379" s="3" t="n">
+        <v>45785.39820251158</v>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="F379" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G379" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H379" t="n">
+        <v>8</v>
+      </c>
+      <c r="I379" t="inlineStr">
+        <is>
+          <t>09:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>shares</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Shares</t>
+        </is>
+      </c>
+      <c r="C380" t="n">
+        <v>2</v>
+      </c>
+      <c r="D380" s="3" t="n">
+        <v>45785.39820251158</v>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="F380" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G380" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H380" t="n">
+        <v>8</v>
+      </c>
+      <c r="I380" t="inlineStr">
+        <is>
+          <t>09:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>saves</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Saves</t>
+        </is>
+      </c>
+      <c r="C381" t="n">
+        <v>3</v>
+      </c>
+      <c r="D381" s="3" t="n">
+        <v>45785.39820251158</v>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="F381" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G381" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H381" t="n">
+        <v>8</v>
+      </c>
+      <c r="I381" t="inlineStr">
+        <is>
+          <t>09:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>replies</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Replies</t>
+        </is>
+      </c>
+      <c r="C382" t="n">
+        <v>1</v>
+      </c>
+      <c r="D382" s="3" t="n">
+        <v>45785.39820251158</v>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="F382" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G382" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H382" t="n">
+        <v>8</v>
+      </c>
+      <c r="I382" t="inlineStr">
+        <is>
+          <t>09:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>views</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Views</t>
+        </is>
+      </c>
+      <c r="C383" t="n">
+        <v>2043</v>
+      </c>
+      <c r="D383" s="3" t="n">
+        <v>45785.39820251158</v>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="F383" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G383" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H383" t="n">
+        <v>8</v>
+      </c>
+      <c r="I383" t="inlineStr">
+        <is>
+          <t>09:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>follows_and_unfollows</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Follows and unfollows</t>
+        </is>
+      </c>
+      <c r="C384" t="n">
+        <v>0</v>
+      </c>
+      <c r="D384" s="3" t="n">
+        <v>45785.39820251158</v>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="F384" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G384" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H384" t="n">
+        <v>8</v>
+      </c>
+      <c r="I384" t="inlineStr">
+        <is>
+          <t>09:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>profile_links_taps</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Profile links taps</t>
+        </is>
+      </c>
+      <c r="C385" t="n">
+        <v>0</v>
+      </c>
+      <c r="D385" s="3" t="n">
+        <v>45785.39820251158</v>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>2025-05-08</t>
+        </is>
+      </c>
+      <c r="F385" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G385" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H385" t="n">
+        <v>8</v>
+      </c>
+      <c r="I385" t="inlineStr">
+        <is>
+          <t>09:33:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>reach</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Accounts reached</t>
+        </is>
+      </c>
+      <c r="C386" t="n">
+        <v>2761</v>
+      </c>
+      <c r="D386" s="3" t="n">
+        <v>45786.39815365741</v>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>2025-05-09</t>
+        </is>
+      </c>
+      <c r="F386" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G386" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H386" t="n">
+        <v>9</v>
+      </c>
+      <c r="I386" t="inlineStr">
+        <is>
+          <t>09:33:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>website_clicks</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Website link taps</t>
+        </is>
+      </c>
+      <c r="C387" t="n">
+        <v>2</v>
+      </c>
+      <c r="D387" s="3" t="n">
+        <v>45786.39815365741</v>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>2025-05-09</t>
+        </is>
+      </c>
+      <c r="F387" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G387" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H387" t="n">
+        <v>9</v>
+      </c>
+      <c r="I387" t="inlineStr">
+        <is>
+          <t>09:33:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>profile_views</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Profile visits</t>
+        </is>
+      </c>
+      <c r="C388" t="n">
+        <v>126</v>
+      </c>
+      <c r="D388" s="3" t="n">
+        <v>45786.39815365741</v>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>2025-05-09</t>
+        </is>
+      </c>
+      <c r="F388" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G388" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H388" t="n">
+        <v>9</v>
+      </c>
+      <c r="I388" t="inlineStr">
+        <is>
+          <t>09:33:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>total_interactions</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Content interactions</t>
+        </is>
+      </c>
+      <c r="C389" t="n">
+        <v>352</v>
+      </c>
+      <c r="D389" s="3" t="n">
+        <v>45786.39815365741</v>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>2025-05-09</t>
+        </is>
+      </c>
+      <c r="F389" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G389" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H389" t="n">
+        <v>9</v>
+      </c>
+      <c r="I389" t="inlineStr">
+        <is>
+          <t>09:33:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>likes</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Likes</t>
+        </is>
+      </c>
+      <c r="C390" t="n">
+        <v>296</v>
+      </c>
+      <c r="D390" s="3" t="n">
+        <v>45786.39815365741</v>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>2025-05-09</t>
+        </is>
+      </c>
+      <c r="F390" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G390" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H390" t="n">
+        <v>9</v>
+      </c>
+      <c r="I390" t="inlineStr">
+        <is>
+          <t>09:33:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="C391" t="n">
+        <v>22</v>
+      </c>
+      <c r="D391" s="3" t="n">
+        <v>45786.39815365741</v>
+      </c>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>2025-05-09</t>
+        </is>
+      </c>
+      <c r="F391" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G391" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H391" t="n">
+        <v>9</v>
+      </c>
+      <c r="I391" t="inlineStr">
+        <is>
+          <t>09:33:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>shares</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Shares</t>
+        </is>
+      </c>
+      <c r="C392" t="n">
+        <v>14</v>
+      </c>
+      <c r="D392" s="3" t="n">
+        <v>45786.39815365741</v>
+      </c>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>2025-05-09</t>
+        </is>
+      </c>
+      <c r="F392" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G392" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H392" t="n">
+        <v>9</v>
+      </c>
+      <c r="I392" t="inlineStr">
+        <is>
+          <t>09:33:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>saves</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Saves</t>
+        </is>
+      </c>
+      <c r="C393" t="n">
+        <v>18</v>
+      </c>
+      <c r="D393" s="3" t="n">
+        <v>45786.39815365741</v>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>2025-05-09</t>
+        </is>
+      </c>
+      <c r="F393" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G393" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H393" t="n">
+        <v>9</v>
+      </c>
+      <c r="I393" t="inlineStr">
+        <is>
+          <t>09:33:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>replies</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Replies</t>
+        </is>
+      </c>
+      <c r="C394" t="n">
+        <v>2</v>
+      </c>
+      <c r="D394" s="3" t="n">
+        <v>45786.39815365741</v>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>2025-05-09</t>
+        </is>
+      </c>
+      <c r="F394" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G394" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H394" t="n">
+        <v>9</v>
+      </c>
+      <c r="I394" t="inlineStr">
+        <is>
+          <t>09:33:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>views</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Views</t>
+        </is>
+      </c>
+      <c r="C395" t="n">
+        <v>4952</v>
+      </c>
+      <c r="D395" s="3" t="n">
+        <v>45786.39815365741</v>
+      </c>
+      <c r="E395" t="inlineStr">
+        <is>
+          <t>2025-05-09</t>
+        </is>
+      </c>
+      <c r="F395" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G395" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H395" t="n">
+        <v>9</v>
+      </c>
+      <c r="I395" t="inlineStr">
+        <is>
+          <t>09:33:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>follows_and_unfollows</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Follows and unfollows</t>
+        </is>
+      </c>
+      <c r="C396" t="n">
+        <v>0</v>
+      </c>
+      <c r="D396" s="3" t="n">
+        <v>45786.39815365741</v>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>2025-05-09</t>
+        </is>
+      </c>
+      <c r="F396" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G396" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H396" t="n">
+        <v>9</v>
+      </c>
+      <c r="I396" t="inlineStr">
+        <is>
+          <t>09:33:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>profile_links_taps</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Profile links taps</t>
+        </is>
+      </c>
+      <c r="C397" t="n">
+        <v>0</v>
+      </c>
+      <c r="D397" s="3" t="n">
+        <v>45786.39815365741</v>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>2025-05-09</t>
+        </is>
+      </c>
+      <c r="F397" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G397" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H397" t="n">
+        <v>9</v>
+      </c>
+      <c r="I397" t="inlineStr">
+        <is>
+          <t>09:33:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>reach</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Accounts reached</t>
+        </is>
+      </c>
+      <c r="C398" t="n">
+        <v>1900</v>
+      </c>
+      <c r="D398" s="3" t="n">
+        <v>45787.39812355324</v>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="F398" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G398" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H398" t="n">
+        <v>10</v>
+      </c>
+      <c r="I398" t="inlineStr">
+        <is>
+          <t>09:33:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>website_clicks</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Website link taps</t>
+        </is>
+      </c>
+      <c r="C399" t="n">
+        <v>4</v>
+      </c>
+      <c r="D399" s="3" t="n">
+        <v>45787.39812355324</v>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="F399" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G399" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H399" t="n">
+        <v>10</v>
+      </c>
+      <c r="I399" t="inlineStr">
+        <is>
+          <t>09:33:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>profile_views</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Profile visits</t>
+        </is>
+      </c>
+      <c r="C400" t="n">
+        <v>104</v>
+      </c>
+      <c r="D400" s="3" t="n">
+        <v>45787.39812355324</v>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="F400" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G400" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H400" t="n">
+        <v>10</v>
+      </c>
+      <c r="I400" t="inlineStr">
+        <is>
+          <t>09:33:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>total_interactions</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Content interactions</t>
+        </is>
+      </c>
+      <c r="C401" t="n">
+        <v>265</v>
+      </c>
+      <c r="D401" s="3" t="n">
+        <v>45787.39812355324</v>
+      </c>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="F401" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G401" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H401" t="n">
+        <v>10</v>
+      </c>
+      <c r="I401" t="inlineStr">
+        <is>
+          <t>09:33:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>likes</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Likes</t>
+        </is>
+      </c>
+      <c r="C402" t="n">
+        <v>201</v>
+      </c>
+      <c r="D402" s="3" t="n">
+        <v>45787.39812355324</v>
+      </c>
+      <c r="E402" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="F402" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G402" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H402" t="n">
+        <v>10</v>
+      </c>
+      <c r="I402" t="inlineStr">
+        <is>
+          <t>09:33:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="C403" t="n">
+        <v>17</v>
+      </c>
+      <c r="D403" s="3" t="n">
+        <v>45787.39812355324</v>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="F403" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G403" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H403" t="n">
+        <v>10</v>
+      </c>
+      <c r="I403" t="inlineStr">
+        <is>
+          <t>09:33:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>shares</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Shares</t>
+        </is>
+      </c>
+      <c r="C404" t="n">
+        <v>7</v>
+      </c>
+      <c r="D404" s="3" t="n">
+        <v>45787.39812355324</v>
+      </c>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="F404" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G404" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H404" t="n">
+        <v>10</v>
+      </c>
+      <c r="I404" t="inlineStr">
+        <is>
+          <t>09:33:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>saves</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Saves</t>
+        </is>
+      </c>
+      <c r="C405" t="n">
+        <v>32</v>
+      </c>
+      <c r="D405" s="3" t="n">
+        <v>45787.39812355324</v>
+      </c>
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="F405" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G405" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H405" t="n">
+        <v>10</v>
+      </c>
+      <c r="I405" t="inlineStr">
+        <is>
+          <t>09:33:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>replies</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Replies</t>
+        </is>
+      </c>
+      <c r="C406" t="n">
+        <v>8</v>
+      </c>
+      <c r="D406" s="3" t="n">
+        <v>45787.39812355324</v>
+      </c>
+      <c r="E406" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="F406" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G406" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H406" t="n">
+        <v>10</v>
+      </c>
+      <c r="I406" t="inlineStr">
+        <is>
+          <t>09:33:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>views</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Views</t>
+        </is>
+      </c>
+      <c r="C407" t="n">
+        <v>3806</v>
+      </c>
+      <c r="D407" s="3" t="n">
+        <v>45787.39812355324</v>
+      </c>
+      <c r="E407" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="F407" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G407" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H407" t="n">
+        <v>10</v>
+      </c>
+      <c r="I407" t="inlineStr">
+        <is>
+          <t>09:33:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>follows_and_unfollows</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Follows and unfollows</t>
+        </is>
+      </c>
+      <c r="C408" t="n">
+        <v>0</v>
+      </c>
+      <c r="D408" s="3" t="n">
+        <v>45787.39812355324</v>
+      </c>
+      <c r="E408" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="F408" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G408" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H408" t="n">
+        <v>10</v>
+      </c>
+      <c r="I408" t="inlineStr">
+        <is>
+          <t>09:33:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>profile_links_taps</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Profile links taps</t>
+        </is>
+      </c>
+      <c r="C409" t="n">
+        <v>0</v>
+      </c>
+      <c r="D409" s="3" t="n">
+        <v>45787.39812355324</v>
+      </c>
+      <c r="E409" t="inlineStr">
+        <is>
+          <t>2025-05-10</t>
+        </is>
+      </c>
+      <c r="F409" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G409" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H409" t="n">
+        <v>10</v>
+      </c>
+      <c r="I409" t="inlineStr">
+        <is>
+          <t>09:33:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>reach</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Accounts reached</t>
+        </is>
+      </c>
+      <c r="C410" t="n">
+        <v>1436</v>
+      </c>
+      <c r="D410" s="3" t="n">
+        <v>45788.39806238426</v>
+      </c>
+      <c r="E410" t="inlineStr">
+        <is>
+          <t>2025-05-11</t>
+        </is>
+      </c>
+      <c r="F410" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G410" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H410" t="n">
+        <v>11</v>
+      </c>
+      <c r="I410" t="inlineStr">
+        <is>
+          <t>09:33:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>website_clicks</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Website link taps</t>
+        </is>
+      </c>
+      <c r="C411" t="n">
+        <v>3</v>
+      </c>
+      <c r="D411" s="3" t="n">
+        <v>45788.39806238426</v>
+      </c>
+      <c r="E411" t="inlineStr">
+        <is>
+          <t>2025-05-11</t>
+        </is>
+      </c>
+      <c r="F411" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G411" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H411" t="n">
+        <v>11</v>
+      </c>
+      <c r="I411" t="inlineStr">
+        <is>
+          <t>09:33:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>profile_views</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Profile visits</t>
+        </is>
+      </c>
+      <c r="C412" t="n">
+        <v>70</v>
+      </c>
+      <c r="D412" s="3" t="n">
+        <v>45788.39806238426</v>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>2025-05-11</t>
+        </is>
+      </c>
+      <c r="F412" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G412" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H412" t="n">
+        <v>11</v>
+      </c>
+      <c r="I412" t="inlineStr">
+        <is>
+          <t>09:33:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>total_interactions</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Content interactions</t>
+        </is>
+      </c>
+      <c r="C413" t="n">
+        <v>291</v>
+      </c>
+      <c r="D413" s="3" t="n">
+        <v>45788.39806238426</v>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>2025-05-11</t>
+        </is>
+      </c>
+      <c r="F413" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G413" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H413" t="n">
+        <v>11</v>
+      </c>
+      <c r="I413" t="inlineStr">
+        <is>
+          <t>09:33:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>likes</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Likes</t>
+        </is>
+      </c>
+      <c r="C414" t="n">
+        <v>237</v>
+      </c>
+      <c r="D414" s="3" t="n">
+        <v>45788.39806238426</v>
+      </c>
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>2025-05-11</t>
+        </is>
+      </c>
+      <c r="F414" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G414" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H414" t="n">
+        <v>11</v>
+      </c>
+      <c r="I414" t="inlineStr">
+        <is>
+          <t>09:33:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="C415" t="n">
+        <v>20</v>
+      </c>
+      <c r="D415" s="3" t="n">
+        <v>45788.39806238426</v>
+      </c>
+      <c r="E415" t="inlineStr">
+        <is>
+          <t>2025-05-11</t>
+        </is>
+      </c>
+      <c r="F415" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G415" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H415" t="n">
+        <v>11</v>
+      </c>
+      <c r="I415" t="inlineStr">
+        <is>
+          <t>09:33:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>shares</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Shares</t>
+        </is>
+      </c>
+      <c r="C416" t="n">
+        <v>10</v>
+      </c>
+      <c r="D416" s="3" t="n">
+        <v>45788.39806238426</v>
+      </c>
+      <c r="E416" t="inlineStr">
+        <is>
+          <t>2025-05-11</t>
+        </is>
+      </c>
+      <c r="F416" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G416" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H416" t="n">
+        <v>11</v>
+      </c>
+      <c r="I416" t="inlineStr">
+        <is>
+          <t>09:33:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>saves</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Saves</t>
+        </is>
+      </c>
+      <c r="C417" t="n">
+        <v>17</v>
+      </c>
+      <c r="D417" s="3" t="n">
+        <v>45788.39806238426</v>
+      </c>
+      <c r="E417" t="inlineStr">
+        <is>
+          <t>2025-05-11</t>
+        </is>
+      </c>
+      <c r="F417" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G417" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H417" t="n">
+        <v>11</v>
+      </c>
+      <c r="I417" t="inlineStr">
+        <is>
+          <t>09:33:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>replies</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Replies</t>
+        </is>
+      </c>
+      <c r="C418" t="n">
+        <v>7</v>
+      </c>
+      <c r="D418" s="3" t="n">
+        <v>45788.39806238426</v>
+      </c>
+      <c r="E418" t="inlineStr">
+        <is>
+          <t>2025-05-11</t>
+        </is>
+      </c>
+      <c r="F418" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G418" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H418" t="n">
+        <v>11</v>
+      </c>
+      <c r="I418" t="inlineStr">
+        <is>
+          <t>09:33:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>views</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Views</t>
+        </is>
+      </c>
+      <c r="C419" t="n">
+        <v>3345</v>
+      </c>
+      <c r="D419" s="3" t="n">
+        <v>45788.39806238426</v>
+      </c>
+      <c r="E419" t="inlineStr">
+        <is>
+          <t>2025-05-11</t>
+        </is>
+      </c>
+      <c r="F419" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G419" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H419" t="n">
+        <v>11</v>
+      </c>
+      <c r="I419" t="inlineStr">
+        <is>
+          <t>09:33:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>follows_and_unfollows</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Follows and unfollows</t>
+        </is>
+      </c>
+      <c r="C420" t="n">
+        <v>0</v>
+      </c>
+      <c r="D420" s="3" t="n">
+        <v>45788.39806238426</v>
+      </c>
+      <c r="E420" t="inlineStr">
+        <is>
+          <t>2025-05-11</t>
+        </is>
+      </c>
+      <c r="F420" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G420" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H420" t="n">
+        <v>11</v>
+      </c>
+      <c r="I420" t="inlineStr">
+        <is>
+          <t>09:33:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>profile_links_taps</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Profile links taps</t>
+        </is>
+      </c>
+      <c r="C421" t="n">
+        <v>0</v>
+      </c>
+      <c r="D421" s="3" t="n">
+        <v>45788.39806238426</v>
+      </c>
+      <c r="E421" t="inlineStr">
+        <is>
+          <t>2025-05-11</t>
+        </is>
+      </c>
+      <c r="F421" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G421" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H421" t="n">
+        <v>11</v>
+      </c>
+      <c r="I421" t="inlineStr">
+        <is>
+          <t>09:33:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>reach</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Accounts reached</t>
+        </is>
+      </c>
+      <c r="C422" t="n">
+        <v>1303</v>
+      </c>
+      <c r="D422" s="3" t="n">
+        <v>45789.42138497146</v>
+      </c>
+      <c r="E422" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="F422" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G422" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H422" t="n">
+        <v>12</v>
+      </c>
+      <c r="I422" t="inlineStr">
+        <is>
+          <t>10:06:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>website_clicks</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Website link taps</t>
+        </is>
+      </c>
+      <c r="C423" t="n">
+        <v>0</v>
+      </c>
+      <c r="D423" s="3" t="n">
+        <v>45789.42138497146</v>
+      </c>
+      <c r="E423" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="F423" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G423" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H423" t="n">
+        <v>12</v>
+      </c>
+      <c r="I423" t="inlineStr">
+        <is>
+          <t>10:06:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>profile_views</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Profile visits</t>
+        </is>
+      </c>
+      <c r="C424" t="n">
+        <v>69</v>
+      </c>
+      <c r="D424" s="3" t="n">
+        <v>45789.42138497146</v>
+      </c>
+      <c r="E424" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="F424" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G424" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H424" t="n">
+        <v>12</v>
+      </c>
+      <c r="I424" t="inlineStr">
+        <is>
+          <t>10:06:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>total_interactions</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Content interactions</t>
+        </is>
+      </c>
+      <c r="C425" t="n">
+        <v>191</v>
+      </c>
+      <c r="D425" s="3" t="n">
+        <v>45789.42138497146</v>
+      </c>
+      <c r="E425" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="F425" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G425" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H425" t="n">
+        <v>12</v>
+      </c>
+      <c r="I425" t="inlineStr">
+        <is>
+          <t>10:06:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>likes</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Likes</t>
+        </is>
+      </c>
+      <c r="C426" t="n">
+        <v>164</v>
+      </c>
+      <c r="D426" s="3" t="n">
+        <v>45789.42138497146</v>
+      </c>
+      <c r="E426" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="F426" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G426" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H426" t="n">
+        <v>12</v>
+      </c>
+      <c r="I426" t="inlineStr">
+        <is>
+          <t>10:06:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="C427" t="n">
+        <v>10</v>
+      </c>
+      <c r="D427" s="3" t="n">
+        <v>45789.42138497146</v>
+      </c>
+      <c r="E427" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="F427" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G427" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H427" t="n">
+        <v>12</v>
+      </c>
+      <c r="I427" t="inlineStr">
+        <is>
+          <t>10:06:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>shares</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Shares</t>
+        </is>
+      </c>
+      <c r="C428" t="n">
+        <v>4</v>
+      </c>
+      <c r="D428" s="3" t="n">
+        <v>45789.42138497146</v>
+      </c>
+      <c r="E428" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="F428" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G428" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H428" t="n">
+        <v>12</v>
+      </c>
+      <c r="I428" t="inlineStr">
+        <is>
+          <t>10:06:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>saves</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Saves</t>
+        </is>
+      </c>
+      <c r="C429" t="n">
+        <v>13</v>
+      </c>
+      <c r="D429" s="3" t="n">
+        <v>45789.42138497146</v>
+      </c>
+      <c r="E429" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="F429" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G429" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H429" t="n">
+        <v>12</v>
+      </c>
+      <c r="I429" t="inlineStr">
+        <is>
+          <t>10:06:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>replies</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Replies</t>
+        </is>
+      </c>
+      <c r="C430" t="n">
+        <v>0</v>
+      </c>
+      <c r="D430" s="3" t="n">
+        <v>45789.42138497146</v>
+      </c>
+      <c r="E430" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="F430" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G430" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H430" t="n">
+        <v>12</v>
+      </c>
+      <c r="I430" t="inlineStr">
+        <is>
+          <t>10:06:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>views</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Views</t>
+        </is>
+      </c>
+      <c r="C431" t="n">
+        <v>2552</v>
+      </c>
+      <c r="D431" s="3" t="n">
+        <v>45789.42138497146</v>
+      </c>
+      <c r="E431" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="F431" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G431" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H431" t="n">
+        <v>12</v>
+      </c>
+      <c r="I431" t="inlineStr">
+        <is>
+          <t>10:06:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>follows_and_unfollows</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Follows and unfollows</t>
+        </is>
+      </c>
+      <c r="C432" t="n">
+        <v>0</v>
+      </c>
+      <c r="D432" s="3" t="n">
+        <v>45789.42138497146</v>
+      </c>
+      <c r="E432" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="F432" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G432" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H432" t="n">
+        <v>12</v>
+      </c>
+      <c r="I432" t="inlineStr">
+        <is>
+          <t>10:06:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>profile_links_taps</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Profile links taps</t>
+        </is>
+      </c>
+      <c r="C433" t="n">
+        <v>0</v>
+      </c>
+      <c r="D433" s="3" t="n">
+        <v>45789.42138497146</v>
+      </c>
+      <c r="E433" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="F433" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G433" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H433" t="n">
+        <v>12</v>
+      </c>
+      <c r="I433" t="inlineStr">
+        <is>
+          <t>10:06:47</t>
         </is>
       </c>
     </row>

</xml_diff>